<commit_message>
reso FullExploration.scala un po' più funzionale
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E617C84-4ECB-43A8-8F6F-2ED8D154DCA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A621B66-62C6-49B4-8869-1C139527E895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Tempo Stimato(Ottimale)</t>
+  </si>
+  <si>
+    <t>Naked Pairs</t>
+  </si>
+  <si>
+    <t>Hidden Pairs</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
-  <dimension ref="B3:H5"/>
+  <dimension ref="B3:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,6 +463,22 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
idea di fare interfaccia alghoritm
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A621B66-62C6-49B4-8869-1C139527E895}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67072A9-AFE3-438D-9201-8B215EE08F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Hidden Pairs</t>
+  </si>
+  <si>
+    <t>Tempo veritiero</t>
+  </si>
+  <si>
+    <t>7gg</t>
   </si>
 </sst>
 </file>
@@ -417,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
-  <dimension ref="B3:H7"/>
+  <dimension ref="B3:I7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -428,9 +434,10 @@
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>3</v>
       </c>
@@ -443,8 +450,11 @@
       <c r="H3" t="s">
         <v>8</v>
       </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -452,7 +462,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -462,8 +472,11 @@
       <c r="H5" t="s">
         <v>7</v>
       </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>9</v>
       </c>
@@ -471,7 +484,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
aggiunti commenti hidden pair
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1805B82B-C462-4AAF-BBA5-C5C78B007CED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6EDDF-6461-4AED-83EF-AFE74AA69017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -468,7 +468,7 @@
   <dimension ref="B3:I15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,6 +617,9 @@
       <c r="C13" t="s">
         <v>21</v>
       </c>
+      <c r="D13" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">

</xml_diff>

<commit_message>
Aggiunta caricamento di vari Sudoku da input, possibilità dell'utente di vedere le possibili liste quando digita un numero sbagliato, controllo sui digits
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37B6EDDF-6461-4AED-83EF-AFE74AA69017}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B65689-8A2E-4210-8839-0D0ADEC75F4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
+    <workbookView xWindow="8700" yWindow="0" windowWidth="10185" windowHeight="10920" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>8gg</t>
+  </si>
+  <si>
+    <t>caricamento vari Sudoku</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
-  <dimension ref="B3:I15"/>
+  <dimension ref="B3:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
@@ -474,7 +477,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
   </cols>
@@ -625,10 +628,21 @@
       <c r="C14" t="s">
         <v>22</v>
       </c>
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunta click su ogni casella (MouseListener)
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AAAA2A0-3A70-46D3-B664-4FB6E0965399}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EA773C-84BF-451C-88E1-138B1BF5AB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
+    <workbookView xWindow="8700" yWindow="0" windowWidth="10185" windowHeight="10920" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="29">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -101,9 +101,6 @@
     <t xml:space="preserve">liste utente </t>
   </si>
   <si>
-    <t>controllo errore</t>
-  </si>
-  <si>
     <t>suggerimento</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>3gg.</t>
+  </si>
+  <si>
+    <t>controllo errori</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
   <dimension ref="B3:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -557,10 +557,10 @@
         <v>5</v>
       </c>
       <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
         <v>25</v>
-      </c>
-      <c r="I8" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
@@ -579,7 +579,7 @@
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
         <v>5</v>
@@ -627,28 +627,40 @@
         <v>5</v>
       </c>
       <c r="H13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
         <v>5</v>
+      </c>
+      <c r="H14" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" t="s">
         <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunta finestra di dialogo quando clicchi su casella
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692F621B-6302-4DE1-B365-B60888A37634}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4662FEB-C67F-4A0D-A0CF-95CBA1DC17CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
   <dimension ref="B3:K25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,7 +709,7 @@
         <v>14</v>
       </c>
       <c r="K23" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
rimesso a posto modulo
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A30BED0-E3BA-4697-BE19-F8AC419BF2C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3C1440-DA0A-4BBD-A12B-E0A99BF44920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4955FB27-693F-426D-8282-B29FF1F7ECAE}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
   <si>
     <t>Algoritmi Risoluzione</t>
   </si>
@@ -137,10 +137,7 @@
     <t>aggiornamento liste</t>
   </si>
   <si>
-    <t>controlli sulla scrittura dei numeri</t>
-  </si>
-  <si>
-    <t>ConfirmDialog di fine gioco</t>
+    <t>controlli sulla scrittura dei numeri/liste e MessageDialog fine gioco</t>
   </si>
 </sst>
 </file>
@@ -494,15 +491,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98DE372D-A862-4253-9190-BE15448DD5CF}">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="19.85546875" customWidth="1"/>
     <col min="3" max="3" width="22.7109375" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="4" max="4" width="60.28515625" customWidth="1"/>
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="15.28515625" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
@@ -712,22 +709,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
-        <v>35</v>
-      </c>
-      <c r="F23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="J24" t="s">
-        <v>14</v>
-      </c>
-      <c r="K24" t="s">
-        <v>15</v>
-      </c>
-    </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
modificato caricamento sudoku, possibilità di aprire giochi in base al livello di difficoltà
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF6C8913-3A2E-4BDF-9FAF-2F538E92184D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72557A-7070-4091-B5DA-EBB957C5375E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Zandoli</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>3gg.</t>
+  </si>
+  <si>
+    <t>5gg</t>
   </si>
 </sst>
 </file>
@@ -492,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -758,10 +761,10 @@
         <v>8</v>
       </c>
       <c r="J26" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>12</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunta nel backog spunta livelli difficoltà
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72557A-7070-4091-B5DA-EBB957C5375E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC9863-7D02-421B-8DDB-74FEABBCBE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Zandoli</t>
   </si>
@@ -495,8 +495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,6 +730,9 @@
       <c r="D22" t="s">
         <v>32</v>
       </c>
+      <c r="F22" t="s">
+        <v>8</v>
+      </c>
       <c r="G22" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
aggiunti sudoku di intermedia difficoltà
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4AC9863-7D02-421B-8DDB-74FEABBCBE23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B642A7-5C6B-4A28-B098-03C8D6C4D886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
   <si>
     <t>Zandoli</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>3gg.</t>
-  </si>
-  <si>
-    <t>5gg</t>
   </si>
 </sst>
 </file>
@@ -495,8 +492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,7 +764,7 @@
         <v>9</v>
       </c>
       <c r="K26" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiunti sudoku di difficile difficoltà
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B642A7-5C6B-4A28-B098-03C8D6C4D886}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94779913-6E02-4876-97C5-B80E0DABAD45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>Zandoli</t>
   </si>
@@ -493,7 +493,7 @@
   <dimension ref="B3:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,8 +730,11 @@
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" t="s">
-        <v>8</v>
+      <c r="J22" t="s">
+        <v>19</v>
+      </c>
+      <c r="K22" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="3:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
settaggio timer e score funzionante
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lorenzo\Documents\UNIBO-Magistrale\ProgettoScala\Sudoku-Scala\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B77BDD59-E37F-463D-8919-F14D121ADCDD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1357D005-3A9E-46D1-845F-EA0D5096BAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
   <si>
     <t>Zandoli</t>
   </si>
@@ -144,7 +144,7 @@
     <t>5gg</t>
   </si>
   <si>
-    <t>salvataggio gioco</t>
+    <t>salvataggio gioco e load gioco</t>
   </si>
 </sst>
 </file>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,6 +773,12 @@
       <c r="D24" t="s">
         <v>39</v>
       </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">

</xml_diff>

<commit_message>
File chooser aggiunti altri impliciti
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1357D005-3A9E-46D1-845F-EA0D5096BAFE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAEF7BC-ECE5-4A0C-A266-38B832E02921}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="40">
   <si>
     <t>Zandoli</t>
   </si>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="C13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -712,6 +712,12 @@
       <c r="F19" t="s">
         <v>8</v>
       </c>
+      <c r="J19" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
@@ -779,6 +785,12 @@
       <c r="G24" t="s">
         <v>8</v>
       </c>
+      <c r="J24" t="s">
+        <v>9</v>
+      </c>
+      <c r="K24" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
@@ -799,7 +811,7 @@
         <v>9</v>
       </c>
       <c r="K27" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sudoku in prolog funzionante
</commit_message>
<xml_diff>
--- a/ProductBacklog.xlsx
+++ b/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\silvi\OneDrive\Desktop\progettoSudoku\progettoSudoku\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680A254B-F4F3-4EA2-9ACF-03C8416CEE44}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B30F52-DCDB-4C47-8DF5-D95F90FBBFFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="43">
   <si>
     <t>Zandoli</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t xml:space="preserve">interfaccia di caricamento vari Sudoku </t>
+  </si>
+  <si>
+    <t>Sudoku in prolog e Engine</t>
   </si>
 </sst>
 </file>
@@ -502,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:K29"/>
+  <dimension ref="B3:K30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -842,6 +845,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="F30" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" t="s">
+        <v>9</v>
+      </c>
+      <c r="K30" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>